<commit_message>
Massive change for whole project.
</commit_message>
<xml_diff>
--- a/Тест-кейсы.xlsx
+++ b/Тест-кейсы.xlsx
@@ -16,15 +16,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="72">
   <si>
     <t xml:space="preserve">Тест-кейсы вкладки Elements -&gt; Web Tables 
 для проекта TOOLSQA (demoqa.com)
 Elements -&gt; Web Tables 
 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Чек-лист про проекту: </t>
   </si>
   <si>
     <t>ID</t>
@@ -362,10 +359,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -373,6 +366,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -684,8 +681,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G48" sqref="A48:G49"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -705,56 +702,54 @@
         <v>0</v>
       </c>
       <c r="B1" s="2"/>
-      <c r="C1" s="3" t="s">
-        <v>1</v>
-      </c>
+      <c r="C1" s="3"/>
     </row>
     <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="D4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="11"/>
+      <c r="G4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" s="5" t="s">
         <v>8</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" s="8"/>
-      <c r="G4" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E5" s="6">
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -762,10 +757,10 @@
         <v>2</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -773,10 +768,10 @@
         <v>3</v>
       </c>
       <c r="F7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -784,10 +779,10 @@
         <v>4</v>
       </c>
       <c r="F8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -795,10 +790,10 @@
         <v>5</v>
       </c>
       <c r="F9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
@@ -806,10 +801,10 @@
         <v>6</v>
       </c>
       <c r="F10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
@@ -817,10 +812,10 @@
         <v>7</v>
       </c>
       <c r="F11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
@@ -828,10 +823,10 @@
         <v>8</v>
       </c>
       <c r="F12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" t="s">
         <v>18</v>
-      </c>
-      <c r="G12" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
@@ -839,30 +834,30 @@
         <v>9</v>
       </c>
       <c r="F13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E15" s="4">
         <v>1</v>
       </c>
       <c r="F15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
@@ -870,10 +865,10 @@
         <v>2</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
@@ -881,10 +876,10 @@
         <v>3</v>
       </c>
       <c r="F17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -892,35 +887,35 @@
         <v>4</v>
       </c>
       <c r="F18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E19" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E21" s="4">
         <v>1</v>
       </c>
       <c r="F21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
@@ -928,10 +923,10 @@
         <v>2</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
@@ -939,10 +934,10 @@
         <v>3</v>
       </c>
       <c r="F23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -950,35 +945,35 @@
         <v>4</v>
       </c>
       <c r="F24" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E25" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B27" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D27" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E27" s="4">
         <v>1</v>
       </c>
       <c r="F27" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
@@ -986,10 +981,10 @@
         <v>2</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G28" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
@@ -997,10 +992,10 @@
         <v>3</v>
       </c>
       <c r="F29" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G29" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -1008,35 +1003,35 @@
         <v>4</v>
       </c>
       <c r="F30" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E31" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
+        <v>34</v>
+      </c>
+      <c r="B33" t="s">
+        <v>21</v>
+      </c>
+      <c r="C33" t="s">
         <v>35</v>
       </c>
-      <c r="B33" t="s">
-        <v>22</v>
-      </c>
-      <c r="C33" t="s">
-        <v>36</v>
-      </c>
       <c r="D33" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E33" s="4">
         <v>1</v>
       </c>
       <c r="F33" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
@@ -1044,10 +1039,10 @@
         <v>2</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G34" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
@@ -1055,22 +1050,22 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B36" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C36" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D36" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E36" s="4">
         <v>1</v>
       </c>
       <c r="F36" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
@@ -1078,30 +1073,30 @@
         <v>2</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G37" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B39" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C39" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D39" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E39" s="4">
         <v>1</v>
       </c>
       <c r="F39" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
@@ -1109,30 +1104,30 @@
         <v>2</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G40" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B42" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C42" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E42" s="4">
         <v>1</v>
       </c>
       <c r="F42" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
@@ -1140,30 +1135,30 @@
         <v>2</v>
       </c>
       <c r="F43" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G43" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B45" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C45" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E45" s="4">
         <v>1</v>
       </c>
       <c r="F45" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
@@ -1171,66 +1166,66 @@
         <v>2</v>
       </c>
       <c r="F46" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G46" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A48" s="9" t="s">
+      <c r="A48" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D48" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="E48" s="9">
+        <v>1</v>
+      </c>
+      <c r="F48" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G48" s="7"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A49" s="7"/>
+      <c r="B49" s="7"/>
+      <c r="C49" s="7"/>
+      <c r="D49" s="7"/>
+      <c r="E49" s="9">
+        <v>2</v>
+      </c>
+      <c r="F49" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="G49" s="7" t="s">
         <v>54</v>
-      </c>
-      <c r="B48" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C48" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="D48" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="E48" s="11">
-        <v>1</v>
-      </c>
-      <c r="F48" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="G48" s="9"/>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A49" s="9"/>
-      <c r="B49" s="9"/>
-      <c r="C49" s="9"/>
-      <c r="D49" s="9"/>
-      <c r="E49" s="11">
-        <v>2</v>
-      </c>
-      <c r="F49" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="G49" s="9" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B51" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C51" t="s">
+        <v>60</v>
+      </c>
+      <c r="D51" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>62</v>
       </c>
       <c r="E51" s="4">
         <v>1</v>
       </c>
       <c r="F51" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
@@ -1238,30 +1233,30 @@
         <v>2</v>
       </c>
       <c r="F52" t="s">
+        <v>62</v>
+      </c>
+      <c r="G52" t="s">
         <v>63</v>
-      </c>
-      <c r="G52" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B54" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C54" t="s">
+        <v>64</v>
+      </c>
+      <c r="D54" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="E54" s="4">
         <v>1</v>
       </c>
       <c r="F54" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
@@ -1269,10 +1264,10 @@
         <v>2</v>
       </c>
       <c r="F55" t="s">
+        <v>62</v>
+      </c>
+      <c r="G55" t="s">
         <v>63</v>
-      </c>
-      <c r="G55" t="s">
-        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>